<commit_message>
Bugfixing vor Start der WIRKLICHEN Tests
-Hauptproblem: Ping hat beim zweiten mal nicht funktioniert, da
	Applikation nicht richtig beendet wurde und daher der UDP Port besetzt war
	(TaskManager abschiessen hilft).
-PILEDSvc wird NICHT mehr benötigt, da ich Performance Problem befürchte, d.h.
Dynamik der Änderung kann nicht ausgewertet, was lt. Schinagl OK ist.
</commit_message>
<xml_diff>
--- a/__Doku/00 Installation Lichtlabor.xlsx
+++ b/__Doku/00 Installation Lichtlabor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Nr</t>
   </si>
@@ -69,13 +69,7 @@
     <t>ControlBox 3</t>
   </si>
   <si>
-    <t>192.168.5.155</t>
-  </si>
-  <si>
     <t>b8:27:eb:56:4c:af</t>
-  </si>
-  <si>
-    <t>Vorraum</t>
   </si>
   <si>
     <t>192.168.5.156</t>
@@ -180,9 +174,6 @@
   </si>
   <si>
     <t>Testraum 2 (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vorraum </t>
   </si>
   <si>
     <t>Versuchleiter Laptop</t>
@@ -194,6 +185,27 @@
     <t>Asus1,:
 User:admin; PW:bitte.vorsicht!
 User:lilab, PW:lilab1234</t>
+  </si>
+  <si>
+    <t>192.168.5.173</t>
+  </si>
+  <si>
+    <t>Zigbee Gruppe</t>
+  </si>
+  <si>
+    <t>TUG_LightLife</t>
+  </si>
+  <si>
+    <t>pw4lightlife</t>
+  </si>
+  <si>
+    <t>Vorraum Box 1</t>
+  </si>
+  <si>
+    <t>Vorraum  Box 2</t>
+  </si>
+  <si>
+    <t>Vorraum Flächenleuchten</t>
   </si>
 </sst>
 </file>
@@ -578,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,10 +602,11 @@
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -607,10 +620,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -621,11 +637,12 @@
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -635,8 +652,9 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -649,11 +667,14 @@
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1">
+        <v>201</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -666,11 +687,12 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -678,207 +700,238 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>211</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1">
+        <v>203</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1">
+        <v>209</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>202</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
+      <c r="A25" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>44</v>
+      <c r="A29" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>